<commit_message>
Merged training result sheet
</commit_message>
<xml_diff>
--- a/tensorflow/columns_experiment/TrainingComparison.xlsx
+++ b/tensorflow/columns_experiment/TrainingComparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\taiga\Documents\GitHub\FacadeAnnotationTool\tensorflow\columns_experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Gen Nishida\Documents\GitHub\FacadeAnnotationTool\tensorflow\columns_experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532D06CF-597A-4246-9125-E5BE75184DDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D794C8-CCB5-4525-8094-E4EE88AE1C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="2805" windowWidth="21945" windowHeight="13125" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,10 +461,10 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -606,17 +606,17 @@
       <c r="G4" s="9">
         <v>60</v>
       </c>
-      <c r="H4" s="5">
-        <v>1.44E-2</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2.9912999999999999E-4</v>
-      </c>
-      <c r="J4" s="6">
-        <v>2.6499999999999999E-2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>3.2000000000000002E-3</v>
+      <c r="H4" s="10">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2.2248E-4</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="K4" s="7">
+        <v>7.4049999999999995E-4</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update FILE_NAME assignment method
</commit_message>
<xml_diff>
--- a/tensorflow/columns_experiment/TrainingComparison.xlsx
+++ b/tensorflow/columns_experiment/TrainingComparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\taiga\Documents\GitHub\FacadeAnnotationTool\tensorflow\columns_experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52872F8-6913-4F14-AFF0-5A649ACFC75C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCAD624-F3D3-4A82-80EE-D548CC4382F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="420" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5805" yWindow="1305" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +148,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -204,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -259,6 +265,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -485,7 +500,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -657,17 +672,17 @@
       <c r="G6" s="9">
         <v>60</v>
       </c>
-      <c r="H6" s="17">
-        <v>1.3899999999999999E-2</v>
-      </c>
-      <c r="I6" s="18">
-        <v>3.1007000000000002E-4</v>
-      </c>
-      <c r="J6" s="19">
-        <v>2.5499999999999998E-2</v>
-      </c>
-      <c r="K6" s="18">
-        <v>1.8E-3</v>
+      <c r="H6" s="20">
+        <v>1.44E-2</v>
+      </c>
+      <c r="I6" s="21">
+        <v>3.3280000000000001E-4</v>
+      </c>
+      <c r="J6" s="22">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="K6" s="21">
+        <v>8.8982000000000004E-4</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">

</xml_diff>